<commit_message>
Updated BOM with battery.
</commit_message>
<xml_diff>
--- a/Hardware/chplex-bom.xlsx
+++ b/Hardware/chplex-bom.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="matrix_badge" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
   <si>
     <t>Reference</t>
   </si>
@@ -179,6 +179,18 @@
   </si>
   <si>
     <t>Totals:</t>
+  </si>
+  <si>
+    <t>BATT</t>
+  </si>
+  <si>
+    <t>CR2032</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/panasonic-bsg/CR2032/P189-ND/31939</t>
+  </si>
+  <si>
+    <t>PRPC003DAAN-RC</t>
   </si>
 </sst>
 </file>
@@ -186,7 +198,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00000"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00000"/>
   </numFmts>
   <fonts count="18">
     <font>
@@ -671,7 +683,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1016,10 +1028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1121,14 +1133,14 @@
         <v>0.34</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G12" si="0">F3*B3</f>
+        <f t="shared" ref="G3:G13" si="0">F3*B3</f>
         <v>0.34</v>
       </c>
       <c r="H3" s="2">
         <v>8.1509999999999999E-2</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" ref="I3:I12" si="1">H3*B3</f>
+        <f t="shared" ref="I3:I13" si="1">H3*B3</f>
         <v>8.1509999999999999E-2</v>
       </c>
       <c r="J3" t="s">
@@ -1216,6 +1228,9 @@
       <c r="D6" t="s">
         <v>16</v>
       </c>
+      <c r="E6" t="s">
+        <v>58</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
@@ -1261,7 +1276,7 @@
         <v>8.3099999999999997E-3</v>
       </c>
       <c r="J7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1295,7 +1310,7 @@
         <v>4.1549999999999997E-2</v>
       </c>
       <c r="J8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1368,71 +1383,99 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="5" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="B11" s="4">
         <v>1</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" t="s">
-        <v>27</v>
+        <v>56</v>
+      </c>
+      <c r="E11" t="s">
+        <v>56</v>
       </c>
       <c r="F11" s="2">
-        <v>0.1598</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="G11" s="2">
-        <f t="shared" si="0"/>
-        <v>0.1598</v>
+        <f t="shared" ref="G11:G12" si="2">F11*B11</f>
+        <v>0.28999999999999998</v>
       </c>
       <c r="H11" s="2">
-        <v>0.1598</v>
+        <v>0.15734000000000001</v>
       </c>
       <c r="I11" s="2">
-        <f t="shared" si="1"/>
-        <v>0.1598</v>
+        <f t="shared" ref="I11:I12" si="3">H11*B11</f>
+        <v>0.15734000000000001</v>
       </c>
       <c r="J11" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B12" s="4">
         <v>1</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.1598</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="2"/>
+        <v>0.1598</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.1598</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="3"/>
+        <v>0.1598</v>
+      </c>
+      <c r="J12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F13" s="2">
         <v>10</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G13" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H13" s="2">
         <v>0.25</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I13" s="2">
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
-      <c r="E14" s="3" t="s">
+    <row r="15" spans="1:10">
+      <c r="E15" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G14" s="2">
-        <f>SUM(G2:G12)</f>
-        <v>19.5398</v>
-      </c>
-      <c r="I14" s="2">
-        <f>SUM(I2:I12)</f>
-        <v>3.2881</v>
+      <c r="G15" s="2">
+        <f>SUM(G2:G13)</f>
+        <v>19.829799999999999</v>
+      </c>
+      <c r="I15" s="2">
+        <f>SUM(I2:I13)</f>
+        <v>3.4454400000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>